<commit_message>
Update Secondary model output 30-4-20.xlsx
</commit_message>
<xml_diff>
--- a/ms/Secondary model output 30-4-20.xlsx
+++ b/ms/Secondary model output 30-4-20.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3972A65-FAE3-E44A-8502-C7432A07D836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC3F669-C9CF-CC4F-8332-F44F0631AEDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="38300" windowHeight="19820" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="19820" xr2:uid="{CEA959A6-D841-5347-BF8F-13749A5754E5}"/>
   </bookViews>
   <sheets>
-    <sheet name="MLMR mod 3 - bird mating system" sheetId="5" r:id="rId1"/>
+    <sheet name="MLMR mod 3 - Mating system" sheetId="5" r:id="rId1"/>
     <sheet name="Secondary mods 1 - Age" sheetId="1" r:id="rId2"/>
     <sheet name="Secondary mods 2 - Population" sheetId="2" r:id="rId3"/>
     <sheet name="Secondary mods 3 - Environment" sheetId="3" r:id="rId4"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="265">
   <si>
     <t>Random Effects Multilevel Models - Personality traits, taxonomic group and age (categorical mod, no interaction term)</t>
   </si>
@@ -694,12 +694,6 @@
     <t>-0.41, 0.38</t>
   </si>
   <si>
-    <t>Random Effects Multilevel Models - Mating system and birds (all personalities)</t>
-  </si>
-  <si>
-    <t>Because we really only have enough mating system data for birds, this model sees how mating system (simplified) moderates overall mean differences in personality and variability in personality</t>
-  </si>
-  <si>
     <t>Important to note that each estimate here is the mean estimate</t>
   </si>
   <si>
@@ -715,9 +709,6 @@
     <t>95% CI</t>
   </si>
   <si>
-    <t>Pred. Interval</t>
-  </si>
-  <si>
     <t>Monogamy</t>
   </si>
   <si>
@@ -764,6 +755,75 @@
   </si>
   <si>
     <t>-0.03, 0.20</t>
+  </si>
+  <si>
+    <t>Random Effects Multilevel Models - Mating system and personality</t>
+  </si>
+  <si>
+    <t>Because we really only have enough mating system data for birds, this model checks how mating system (simplified) moderates overall mean differences in personality and variability in personality</t>
+  </si>
+  <si>
+    <t>p=0.8</t>
+  </si>
+  <si>
+    <t>-0.33, 0.47</t>
+  </si>
+  <si>
+    <t>-0.36, 0.33</t>
+  </si>
+  <si>
+    <t>p=0.42</t>
+  </si>
+  <si>
+    <t>-0.35, 0.71</t>
+  </si>
+  <si>
+    <t>-0.10, 0.49</t>
+  </si>
+  <si>
+    <t>-0.56, 0.43</t>
+  </si>
+  <si>
+    <t>-0.34, 0.52</t>
+  </si>
+  <si>
+    <t>p=0.58</t>
+  </si>
+  <si>
+    <t>-0.39, 0.89</t>
+  </si>
+  <si>
+    <t>-0.38, 0.21</t>
+  </si>
+  <si>
+    <t>-0.21, 0.08</t>
+  </si>
+  <si>
+    <t>-0.07, 0.06</t>
+  </si>
+  <si>
+    <t>p=0.66</t>
+  </si>
+  <si>
+    <t>-0.38, 0.29</t>
+  </si>
+  <si>
+    <t>-0.13, 0.05</t>
+  </si>
+  <si>
+    <t>-0.25, 0.29</t>
+  </si>
+  <si>
+    <t>-0.15, 0.30</t>
+  </si>
+  <si>
+    <t>p=0.96</t>
+  </si>
+  <si>
+    <t>-0.55, 0.38</t>
+  </si>
+  <si>
+    <t>-0.18, 0.26</t>
   </si>
 </sst>
 </file>
@@ -1235,39 +1295,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9948B2D6-0D24-AC4F-B3C7-22D23935FFEB}">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:AN60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="AO29" sqref="AO29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1278,14 +1343,65 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -1295,8 +1411,44 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>1775.98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7">
+        <v>1935.16</v>
+      </c>
+      <c r="S7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z7">
+        <v>2207.65</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH7">
+        <v>77.37</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1304,11 +1456,47 @@
         <v>0.33</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8">
+        <v>0.88</v>
+      </c>
+      <c r="S8" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="AA8" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AG8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH8" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AI8" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
@@ -1319,9 +1507,48 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>20</v>
@@ -1330,15 +1557,70 @@
         <v>21</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10" s="9"/>
+      <c r="J10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="10"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1352,10 +1634,59 @@
         <v>51</v>
       </c>
       <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11">
+        <v>0.03</v>
+      </c>
+      <c r="K11">
+        <v>0.17</v>
+      </c>
+      <c r="L11">
+        <v>42</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11">
+        <v>0.9</v>
+      </c>
+      <c r="S11">
+        <v>0.95</v>
+      </c>
+      <c r="T11">
+        <v>43</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="Y11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z11">
+        <v>0.1</v>
+      </c>
+      <c r="AA11">
+        <v>0.32</v>
+      </c>
+      <c r="AB11">
+        <v>59</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH11">
+        <v>1E-3</v>
+      </c>
+      <c r="AI11">
+        <v>0.03</v>
+      </c>
+      <c r="AJ11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1366,8 +1697,56 @@
       <c r="D12">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>0.05</v>
+      </c>
+      <c r="K12">
+        <v>0.22</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>35</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z12">
+        <v>0.12</v>
+      </c>
+      <c r="AA12">
+        <v>0.35</v>
+      </c>
+      <c r="AB12">
+        <v>41</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH12">
+        <v>0.06</v>
+      </c>
+      <c r="AI12">
+        <v>0.24</v>
+      </c>
+      <c r="AJ12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1380,8 +1759,56 @@
       <c r="D13">
         <v>503</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13">
+        <v>0.16</v>
+      </c>
+      <c r="K13">
+        <v>0.4</v>
+      </c>
+      <c r="L13">
+        <v>488</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>25</v>
+      </c>
+      <c r="R13">
+        <v>0.12</v>
+      </c>
+      <c r="S13">
+        <v>0.34</v>
+      </c>
+      <c r="T13">
+        <v>436</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z13">
+        <v>0.17</v>
+      </c>
+      <c r="AA13">
+        <v>0.41</v>
+      </c>
+      <c r="AB13">
+        <v>648</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH13">
+        <v>0.02</v>
+      </c>
+      <c r="AI13">
+        <v>0.15</v>
+      </c>
+      <c r="AJ13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
@@ -1392,38 +1819,162 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E15" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="E15" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="F15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="N15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="O15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="P15" s="10" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="X15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF15" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN15" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B16">
         <v>-0.1</v>
@@ -1431,56 +1982,258 @@
       <c r="C16" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16">
+        <v>-0.81</v>
+      </c>
       <c r="E16">
-        <v>-0.81</v>
-      </c>
-      <c r="F16">
         <v>0.42</v>
       </c>
+      <c r="F16" s="32">
+        <v>387</v>
+      </c>
       <c r="G16" s="32">
-        <v>387</v>
+        <v>93</v>
       </c>
       <c r="H16" s="32">
-        <v>93</v>
-      </c>
-      <c r="I16" s="32">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>226</v>
+      </c>
+      <c r="J16" s="29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="L16" s="29">
+        <v>0.36</v>
+      </c>
+      <c r="M16" s="29">
+        <v>0.72</v>
+      </c>
+      <c r="N16" s="29">
+        <v>65</v>
+      </c>
+      <c r="O16" s="29">
+        <v>5</v>
+      </c>
+      <c r="P16" s="29">
+        <v>8</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>226</v>
+      </c>
+      <c r="R16">
+        <v>0.18</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="T16">
+        <v>0.68</v>
+      </c>
+      <c r="U16">
+        <v>0.5</v>
+      </c>
+      <c r="V16">
+        <v>24</v>
+      </c>
+      <c r="W16">
+        <v>3</v>
+      </c>
+      <c r="X16">
+        <v>3</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z16" s="6">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="AA16" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB16" s="6">
+        <v>-0.27</v>
+      </c>
+      <c r="AC16" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>109</v>
+      </c>
+      <c r="AE16" s="6">
+        <v>8</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>9</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH16" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="AI16" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ16" s="29">
+        <v>0.77</v>
+      </c>
+      <c r="AK16" s="29">
+        <v>0.44</v>
+      </c>
+      <c r="AL16" s="29">
+        <v>2</v>
+      </c>
+      <c r="AM16" s="29">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B17" s="14">
         <v>-0.05</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" s="15"/>
+        <v>228</v>
+      </c>
+      <c r="D17" s="14">
+        <v>-0.24</v>
+      </c>
       <c r="E17" s="14">
-        <v>-0.24</v>
+        <v>0.81</v>
       </c>
       <c r="F17" s="14">
-        <v>0.81</v>
+        <v>116</v>
       </c>
       <c r="G17" s="14">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="H17" s="14">
-        <v>12</v>
-      </c>
-      <c r="I17" s="14">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I17" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="J17" s="14">
+        <v>-0.02</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="L17" s="14">
+        <v>-0.1</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0.92</v>
+      </c>
+      <c r="N17" s="14">
+        <v>423</v>
+      </c>
+      <c r="O17" s="16">
+        <v>15</v>
+      </c>
+      <c r="P17" s="14">
+        <v>34</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="R17" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="S17" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="T17" s="16">
+        <v>1.33</v>
+      </c>
+      <c r="U17" s="16">
+        <v>0.19</v>
+      </c>
+      <c r="V17" s="16">
+        <v>412</v>
+      </c>
+      <c r="W17" s="16">
+        <v>33</v>
+      </c>
+      <c r="X17" s="16">
+        <v>41</v>
+      </c>
+      <c r="Y17" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z17" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="AA17" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB17" s="14">
+        <v>0.43</v>
+      </c>
+      <c r="AC17" s="14">
+        <v>0.67</v>
+      </c>
+      <c r="AD17" s="14">
+        <v>539</v>
+      </c>
+      <c r="AE17" s="14">
+        <v>33</v>
+      </c>
+      <c r="AF17" s="14">
+        <v>52</v>
+      </c>
+      <c r="AG17" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH17" s="16">
+        <v>-0.08</v>
+      </c>
+      <c r="AI17" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ17" s="16">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="AK17" s="16">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AL17" s="14">
+        <v>53</v>
+      </c>
+      <c r="AM17" s="14">
+        <v>6</v>
+      </c>
+      <c r="AN17" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG18" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
@@ -1490,8 +2243,44 @@
       <c r="C19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>973.96</v>
+      </c>
+      <c r="K19" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>1125.44</v>
+      </c>
+      <c r="S19" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z19">
+        <v>1015.04</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH19">
+        <v>36.46</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
@@ -1499,10 +2288,46 @@
         <v>0.2</v>
       </c>
       <c r="C20" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R20">
+        <v>0.42</v>
+      </c>
+      <c r="S20" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z20">
+        <v>0.35</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>209</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
@@ -1513,9 +2338,48 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+      <c r="AN21" s="8"/>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="10" t="s">
         <v>20</v>
@@ -1524,15 +2388,70 @@
         <v>21</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I22" s="9"/>
+      <c r="J22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="10"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="10"/>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1545,10 +2464,58 @@
       <c r="D23" s="6">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23">
+        <v>0.01</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="L23">
+        <v>42</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>23</v>
+      </c>
+      <c r="R23">
+        <v>0.05</v>
+      </c>
+      <c r="S23">
+        <v>0.22</v>
+      </c>
+      <c r="T23">
+        <v>43</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z23">
+        <v>0.04</v>
+      </c>
+      <c r="AA23">
+        <v>0.19</v>
+      </c>
+      <c r="AB23">
+        <v>59</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B24">
         <v>0.36</v>
@@ -1559,8 +2526,57 @@
       <c r="D24">
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>20</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>35</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z24">
+        <v>0.03</v>
+      </c>
+      <c r="AA24">
+        <v>0.18</v>
+      </c>
+      <c r="AB24">
+        <v>41</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH24">
+        <v>0.02</v>
+      </c>
+      <c r="AI24">
+        <v>0.15</v>
+      </c>
+      <c r="AJ24">
+        <v>7</v>
+      </c>
+      <c r="AK24" s="5"/>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1573,8 +2589,56 @@
       <c r="D25">
         <v>503</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25">
+        <v>0.1</v>
+      </c>
+      <c r="K25">
+        <v>0.32</v>
+      </c>
+      <c r="L25">
+        <v>488</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>25</v>
+      </c>
+      <c r="R25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S25">
+        <v>0.27</v>
+      </c>
+      <c r="T25">
+        <v>436</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z25">
+        <v>0.03</v>
+      </c>
+      <c r="AA25">
+        <v>0.18</v>
+      </c>
+      <c r="AB25">
+        <v>648</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
+        <v>0</v>
+      </c>
+      <c r="AJ25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -1585,109 +2649,414 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH26" s="8"/>
+      <c r="AI26" s="8"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8"/>
+      <c r="AN26" s="8"/>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="E27" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F27" t="s">
+      <c r="E27" t="s">
         <v>29</v>
       </c>
+      <c r="F27" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="G27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="O27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="P27" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="K27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="U27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="V27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="X27" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN27" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B28" s="8">
         <v>-0.17</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D28" s="18"/>
+        <v>231</v>
+      </c>
+      <c r="D28" s="8">
+        <v>-0.63</v>
+      </c>
       <c r="E28" s="8">
-        <v>-0.63</v>
-      </c>
-      <c r="F28" s="8">
         <v>0.53</v>
       </c>
+      <c r="F28" s="32">
+        <v>387</v>
+      </c>
       <c r="G28" s="32">
-        <v>387</v>
+        <v>93</v>
       </c>
       <c r="H28" s="32">
-        <v>93</v>
-      </c>
-      <c r="I28" s="32">
         <v>44</v>
       </c>
-      <c r="K28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>226</v>
+      </c>
+      <c r="J28" s="27">
+        <v>-0.06</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="L28" s="27">
+        <v>-0.85</v>
+      </c>
+      <c r="M28" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="N28" s="29">
+        <v>65</v>
+      </c>
+      <c r="O28" s="29">
+        <v>5</v>
+      </c>
+      <c r="P28" s="29">
+        <v>8</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>226</v>
+      </c>
+      <c r="R28">
+        <v>-0.05</v>
+      </c>
+      <c r="S28" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="T28">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="U28">
+        <v>0.78</v>
+      </c>
+      <c r="V28">
+        <v>24</v>
+      </c>
+      <c r="W28">
+        <v>3</v>
+      </c>
+      <c r="X28">
+        <v>3</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z28" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="AA28" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB28" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AC28" s="8">
+        <v>0.89</v>
+      </c>
+      <c r="AD28" s="6">
+        <v>109</v>
+      </c>
+      <c r="AE28" s="6">
+        <v>8</v>
+      </c>
+      <c r="AF28" s="6">
+        <v>9</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH28" s="8">
+        <v>-0.08</v>
+      </c>
+      <c r="AI28" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="AJ28" s="8">
+        <v>-0.36</v>
+      </c>
+      <c r="AK28" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="AL28" s="29">
+        <v>2</v>
+      </c>
+      <c r="AM28" s="29">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B29" s="16">
         <v>-0.15</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" s="16">
+        <v>-0.48</v>
+      </c>
+      <c r="E29" s="16">
+        <v>0.63</v>
+      </c>
+      <c r="F29" s="14">
+        <v>116</v>
+      </c>
+      <c r="G29" s="14">
+        <v>12</v>
+      </c>
+      <c r="H29" s="14">
+        <v>9</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="J29" s="14">
+        <v>-0.01</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="L29" s="14">
+        <v>-0.22</v>
+      </c>
+      <c r="M29" s="14">
+        <v>0.83</v>
+      </c>
+      <c r="N29" s="14">
+        <v>423</v>
+      </c>
+      <c r="O29" s="16">
+        <v>15</v>
+      </c>
+      <c r="P29" s="14">
+        <v>34</v>
+      </c>
+      <c r="Q29" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="R29" s="16">
+        <v>-0.04</v>
+      </c>
+      <c r="S29" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="T29" s="16">
+        <v>-0.89</v>
+      </c>
+      <c r="U29" s="16">
+        <v>0.37</v>
+      </c>
+      <c r="V29" s="16">
+        <v>412</v>
+      </c>
+      <c r="W29" s="16">
+        <v>33</v>
+      </c>
+      <c r="X29" s="16">
+        <v>41</v>
+      </c>
+      <c r="Y29" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z29" s="16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA29" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB29" s="16">
+        <v>0.64</v>
+      </c>
+      <c r="AC29" s="16">
+        <v>0.52</v>
+      </c>
+      <c r="AD29" s="14">
+        <v>539</v>
+      </c>
+      <c r="AE29" s="14">
+        <v>33</v>
+      </c>
+      <c r="AF29" s="14">
+        <v>52</v>
+      </c>
+      <c r="AG29" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH29" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="AI29" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ29" s="16">
+        <v>0.34</v>
+      </c>
+      <c r="AK29" s="16">
+        <v>0.73</v>
+      </c>
+      <c r="AL29" s="14">
+        <v>53</v>
+      </c>
+      <c r="AM29" s="14">
+        <v>6</v>
+      </c>
+      <c r="AN29" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>236</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="16">
-        <v>-0.48</v>
-      </c>
-      <c r="F29" s="16">
-        <v>0.63</v>
-      </c>
-      <c r="G29" s="14">
-        <v>116</v>
-      </c>
-      <c r="H29" s="14">
-        <v>12</v>
-      </c>
-      <c r="I29" s="14">
-        <v>9</v>
-      </c>
-      <c r="K29" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1698,14 +3067,13 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>10</v>
       </c>
@@ -1716,7 +3084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>13</v>
       </c>
@@ -1724,11 +3092,11 @@
         <v>0.27</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>19</v>
       </c>
@@ -1739,9 +3107,8 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="10" t="s">
         <v>20</v>
@@ -1750,15 +3117,14 @@
         <v>21</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1773,9 +3139,9 @@
       </c>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1787,7 +3153,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1801,7 +3167,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>26</v>
       </c>
@@ -1812,95 +3178,89 @@
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E43" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="E43" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="F43" s="10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I43" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B44">
         <v>-0.19</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="D44" s="11"/>
+        <v>238</v>
+      </c>
+      <c r="D44">
+        <v>-0.68</v>
+      </c>
       <c r="E44">
-        <v>-0.68</v>
-      </c>
-      <c r="F44">
         <v>0.5</v>
       </c>
+      <c r="F44" s="32">
+        <v>217</v>
+      </c>
       <c r="G44" s="32">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="H44" s="32">
-        <v>83</v>
-      </c>
-      <c r="I44" s="32">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B45" s="14">
         <v>-0.11</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D45" s="15"/>
+        <v>239</v>
+      </c>
+      <c r="D45" s="14">
+        <v>-0.36</v>
+      </c>
       <c r="E45" s="14">
-        <v>-0.36</v>
+        <v>0.72</v>
       </c>
       <c r="F45" s="14">
-        <v>0.72</v>
+        <v>44</v>
       </c>
       <c r="G45" s="14">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H45" s="14">
-        <v>11</v>
-      </c>
-      <c r="I45" s="14">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>10</v>
       </c>
@@ -1911,7 +3271,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>13</v>
       </c>
@@ -1922,7 +3282,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>19</v>
       </c>
@@ -1933,9 +3293,8 @@
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
       <c r="B50" s="10" t="s">
         <v>20</v>
@@ -1944,15 +3303,14 @@
         <v>21</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1966,9 +3324,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B52">
         <v>5.0000000000000001E-3</v>
@@ -1980,7 +3338,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -1994,7 +3352,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>26</v>
       </c>
@@ -2005,86 +3363,95 @@
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>20</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="E55" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="D55" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F55" t="s">
+      <c r="E55" t="s">
         <v>29</v>
       </c>
+      <c r="F55" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="G55" s="10" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I55" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B56" s="8">
         <v>0.05</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="D56" s="18"/>
+        <v>240</v>
+      </c>
+      <c r="D56" s="8">
+        <v>1.27</v>
+      </c>
       <c r="E56" s="8">
-        <v>1.27</v>
-      </c>
-      <c r="F56" s="8">
         <v>0.21</v>
       </c>
+      <c r="F56" s="32">
+        <v>217</v>
+      </c>
       <c r="G56" s="32">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="H56" s="32">
-        <v>83</v>
-      </c>
-      <c r="I56" s="32">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B57" s="16">
         <v>0.08</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D57" s="17"/>
+        <v>241</v>
+      </c>
+      <c r="D57" s="16">
+        <v>1.4</v>
+      </c>
       <c r="E57" s="16">
-        <v>1.4</v>
-      </c>
-      <c r="F57" s="16">
         <v>0.16</v>
       </c>
+      <c r="F57" s="14">
+        <v>44</v>
+      </c>
       <c r="G57" s="14">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H57" s="14">
-        <v>11</v>
-      </c>
-      <c r="I57" s="14">
         <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +3464,7 @@
   <dimension ref="A1:AN67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AO29" sqref="AO29"/>
+      <selection activeCell="I5" sqref="I5:AN29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7863,7 +9230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FBA234-D4FE-CE44-A5C8-7BF7641E4438}">
   <dimension ref="A1:AN29"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>